<commit_message>
Updated reader file and data
</commit_message>
<xml_diff>
--- a/new-backend/matrix.xlsx
+++ b/new-backend/matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\degle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\degle\Google Drive\Hep Tool\Django_AnalysisTool\new-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="645" yWindow="915" windowWidth="28155" windowHeight="16740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gender" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="60">
   <si>
     <t>HCC</t>
   </si>
@@ -220,12 +220,6 @@
     <t>age 2</t>
   </si>
   <si>
-    <t>age 3</t>
-  </si>
-  <si>
-    <t>mort 1</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -238,10 +232,13 @@
     <t>Inactive and HBsAg loss</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
+    <t>Male then Female</t>
+  </si>
+  <si>
+    <t>age 0</t>
+  </si>
+  <si>
+    <t>mort 0</t>
   </si>
 </sst>
 </file>
@@ -354,14 +351,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77043072-7561-4A8D-A6F0-FE15417FB6ED}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -657,13 +654,13 @@
     <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="5" width="23.5" customWidth="1"/>
     <col min="6" max="6" width="7.875" customWidth="1"/>
-    <col min="8" max="8" width="17.625" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="10" width="22.375" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="8" max="9" width="17.625" customWidth="1"/>
+    <col min="10" max="10" width="23.375" customWidth="1"/>
+    <col min="11" max="11" width="22.375" customWidth="1"/>
+    <col min="12" max="12" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
@@ -689,334 +686,350 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14">
         <v>1</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14">
         <v>1</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14">
         <v>1</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="8"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14">
         <v>1</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14">
         <v>1</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <v>1</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14">
         <v>1</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="8"/>
+      <c r="N3" s="14"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>1</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <v>1</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14">
         <v>1</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="14"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14">
         <v>1</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14">
         <v>1</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14">
         <v>1</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="8"/>
+      <c r="N5" s="14"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14">
         <v>1</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
         <v>1</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15">
         <v>1</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>1</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14">
         <v>1</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14">
         <v>1</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="8"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14">
         <v>1</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15">
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14">
         <v>1</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="8"/>
+      <c r="N9" s="14"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
         <v>1</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="8"/>
+      <c r="N10" s="14"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14">
         <v>1</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="8"/>
+      <c r="N11" s="14"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14">
         <v>1</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14">
         <v>1</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="8"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="8"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="8"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1025,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFB8956-2854-4AF1-8456-FE2920426C86}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1039,13 +1052,13 @@
     <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="5" width="23.5" customWidth="1"/>
     <col min="6" max="6" width="7.875" customWidth="1"/>
-    <col min="8" max="8" width="17.625" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="10" width="22.375" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="8" max="9" width="17.625" customWidth="1"/>
+    <col min="10" max="10" width="23.375" customWidth="1"/>
+    <col min="11" max="11" width="22.375" customWidth="1"/>
+    <col min="12" max="12" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
@@ -1071,394 +1084,410 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14">
         <v>1.6E-2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14">
         <v>1.47E-2</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L2" s="15">
+      <c r="M2" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="M2" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <v>1.6E-2</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L3" s="15">
+      <c r="M3" s="14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="M3" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" s="8"/>
+      <c r="N3" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14">
         <v>3.9E-2</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <v>6.3E-2</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L4" s="15">
+      <c r="M4" s="14">
         <v>4.8899999999999999E-2</v>
       </c>
-      <c r="M4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="8"/>
+      <c r="N4" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14">
         <v>1.2E-2</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14">
         <v>0.15</v>
       </c>
-      <c r="M5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="8"/>
+      <c r="N5" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
         <v>0.151</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="8"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14">
         <v>0.01</v>
       </c>
-      <c r="L8" s="15">
+      <c r="M8" s="14">
         <v>2.4400000000000002E-2</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" s="8"/>
+      <c r="N8" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15">
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="M9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" s="8"/>
+      <c r="N9" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
         <v>0.17</v>
       </c>
-      <c r="M10" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" s="8"/>
+      <c r="N10" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14">
         <v>0.16</v>
       </c>
-      <c r="M11" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="8"/>
+      <c r="N11" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14">
         <v>2.8E-3</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14">
         <v>9.1E-4</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="N12" s="8"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="8"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1482,16 +1511,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1538,7 +1567,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2039,1122 +2068,1322 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E97F72-573C-4AC2-A67C-81C81E8B485F}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>4.4499999999999997E-4</v>
       </c>
-      <c r="C2">
-        <v>3.8200000000000002E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3.01E-4</v>
       </c>
-      <c r="C3">
-        <v>2.2499999999999999E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2.4000000000000001E-4</v>
       </c>
-      <c r="C4">
-        <v>1.75E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1.83E-4</v>
       </c>
-      <c r="C5">
-        <v>1.5100000000000001E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1.6899999999999999E-4</v>
       </c>
-      <c r="C6">
-        <v>1.3200000000000001E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="C7">
-        <v>1.17E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>1.34E-4</v>
       </c>
-      <c r="C8">
-        <v>1.06E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>1.15E-4</v>
       </c>
-      <c r="C9">
-        <v>9.6000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>9.7E-5</v>
       </c>
-      <c r="C10">
-        <v>8.7999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>8.5000000000000006E-5</v>
       </c>
-      <c r="C11">
-        <v>8.3999999999999995E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>9.2E-5</v>
       </c>
-      <c r="C12">
-        <v>8.7000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>1.3200000000000001E-4</v>
       </c>
-      <c r="C13">
-        <v>1.02E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2.13E-4</v>
       </c>
-      <c r="C14">
-        <v>1.2899999999999999E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>3.2299999999999999E-4</v>
       </c>
-      <c r="C15">
-        <v>1.66E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>4.3899999999999999E-4</v>
       </c>
-      <c r="C16">
-        <v>2.0699999999999999E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>5.5199999999999997E-4</v>
       </c>
-      <c r="C17">
-        <v>2.4699999999999999E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>6.7500000000000004E-4</v>
       </c>
-      <c r="C18">
-        <v>2.8600000000000001E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>8.0699999999999999E-4</v>
       </c>
-      <c r="C19">
-        <v>3.2000000000000003E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>9.4200000000000002E-4</v>
       </c>
-      <c r="C20">
-        <v>3.5100000000000002E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>1.085E-3</v>
       </c>
-      <c r="C21">
-        <v>3.8400000000000001E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>1.2160000000000001E-3</v>
       </c>
-      <c r="C22">
-        <v>4.1599999999999997E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>1.31E-3</v>
       </c>
-      <c r="C23">
-        <v>4.4499999999999997E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>1.353E-3</v>
       </c>
-      <c r="C24">
-        <v>4.6700000000000002E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>1.358E-3</v>
       </c>
-      <c r="C25">
-        <v>4.86E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>1.351E-3</v>
       </c>
-      <c r="C26">
-        <v>5.0500000000000002E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>1.3489999999999999E-3</v>
       </c>
-      <c r="C27">
-        <v>5.2599999999999999E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>1.353E-3</v>
       </c>
-      <c r="C28">
-        <v>5.53E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>1.371E-3</v>
       </c>
-      <c r="C29">
-        <v>5.8699999999999996E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>1.3990000000000001E-3</v>
       </c>
-      <c r="C30">
-        <v>6.2699999999999995E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>1.4319999999999999E-3</v>
       </c>
-      <c r="C31">
-        <v>6.7299999999999999E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>1.464E-3</v>
       </c>
-      <c r="C32">
-        <v>7.2099999999999996E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>1.4959999999999999E-3</v>
       </c>
-      <c r="C33">
-        <v>7.6599999999999997E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>1.5280000000000001E-3</v>
       </c>
-      <c r="C34">
-        <v>8.0500000000000005E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>1.5629999999999999E-3</v>
       </c>
-      <c r="C35">
-        <v>8.4199999999999998E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>1.6130000000000001E-3</v>
       </c>
-      <c r="C36">
-        <v>8.8800000000000001E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>1.6819999999999999E-3</v>
       </c>
-      <c r="C37">
-        <v>9.4700000000000003E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>1.7639999999999999E-3</v>
       </c>
-      <c r="C38">
-        <v>1.0169999999999999E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>1.8569999999999999E-3</v>
       </c>
-      <c r="C39">
-        <v>1.0989999999999999E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>1.964E-3</v>
       </c>
-      <c r="C40">
-        <v>1.1919999999999999E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>2.0830000000000002E-3</v>
       </c>
-      <c r="C41">
-        <v>1.291E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>2.2269999999999998E-3</v>
       </c>
-      <c r="C42">
-        <v>1.402E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>2.4139999999999999E-3</v>
       </c>
-      <c r="C43">
-        <v>1.5349999999999999E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>2.653E-3</v>
       </c>
-      <c r="C44">
-        <v>1.6949999999999999E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>2.9390000000000002E-3</v>
       </c>
-      <c r="C45">
-        <v>1.879E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>3.2429999999999998E-3</v>
       </c>
-      <c r="C46">
-        <v>2.0699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>3.5630000000000002E-3</v>
       </c>
-      <c r="C47">
-        <v>2.2680000000000001E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>3.9220000000000001E-3</v>
       </c>
-      <c r="C48">
-        <v>2.4859999999999999E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>4.3200000000000001E-3</v>
       </c>
-      <c r="C49">
-        <v>2.725E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>4.7489999999999997E-3</v>
       </c>
-      <c r="C50">
-        <v>2.977E-3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>5.1929999999999997E-3</v>
       </c>
-      <c r="C51">
-        <v>3.2450000000000001E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>5.6470000000000001E-3</v>
       </c>
-      <c r="C52">
-        <v>3.5140000000000002E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <v>6.1219999999999998E-3</v>
       </c>
-      <c r="C53">
-        <v>3.7759999999999998E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
         <v>6.6299999999999996E-3</v>
       </c>
-      <c r="C54">
-        <v>4.0289999999999996E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <v>7.1809999999999999E-3</v>
       </c>
-      <c r="C55">
-        <v>4.2890000000000003E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
         <v>7.7790000000000003E-3</v>
       </c>
-      <c r="C56">
-        <v>4.5640000000000003E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
         <v>8.4150000000000006E-3</v>
       </c>
-      <c r="C57">
-        <v>4.875E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
         <v>9.0740000000000005E-3</v>
       </c>
-      <c r="C58">
-        <v>5.2339999999999999E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
         <v>9.7269999999999995E-3</v>
       </c>
-      <c r="C59">
-        <v>5.6470000000000001E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
         <v>1.0371E-2</v>
       </c>
-      <c r="C60">
-        <v>6.1029999999999999E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
         <v>1.1034E-2</v>
       </c>
-      <c r="C61">
-        <v>6.5890000000000002E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <v>1.1738E-2</v>
       </c>
-      <c r="C62">
-        <v>7.1040000000000001E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <v>1.2489E-2</v>
       </c>
-      <c r="C63">
-        <v>7.6649999999999999E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
         <v>1.3335E-2</v>
       </c>
-      <c r="C64">
-        <v>8.3029999999999996E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <v>1.4319E-2</v>
       </c>
-      <c r="C65">
-        <v>9.0500000000000008E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
         <v>1.5481999999999999E-2</v>
       </c>
-      <c r="C66">
-        <v>9.953E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
         <v>1.6823999999999999E-2</v>
       </c>
-      <c r="C67">
-        <v>1.1001E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
         <v>1.8329999999999999E-2</v>
       </c>
-      <c r="C68">
-        <v>1.2123999999999999E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
         <v>1.9900000000000001E-2</v>
       </c>
-      <c r="C69">
-        <v>1.325E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
         <v>2.1538999999999999E-2</v>
       </c>
-      <c r="C70">
-        <v>1.4419E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
         <v>2.3396E-2</v>
       </c>
-      <c r="C71">
-        <v>1.5717999999999999E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
         <v>2.5475999999999999E-2</v>
       </c>
-      <c r="C72">
-        <v>1.7201000000000001E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
         <v>2.7793999999999999E-2</v>
       </c>
-      <c r="C73">
-        <v>1.8896E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
         <v>3.0349999999999999E-2</v>
       </c>
-      <c r="C74">
-        <v>2.0818E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
         <v>3.3203999999999997E-2</v>
       </c>
-      <c r="C75">
-        <v>2.2995999999999999E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
         <v>3.6345000000000002E-2</v>
       </c>
-      <c r="C76">
-        <v>2.5387E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
         <v>3.9787999999999997E-2</v>
       </c>
-      <c r="C77">
-        <v>2.809E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
         <v>4.3720000000000002E-2</v>
       </c>
-      <c r="C78">
-        <v>3.1224999999999999E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
         <v>4.8335000000000003E-2</v>
       </c>
-      <c r="C79">
-        <v>3.4785999999999997E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
         <v>5.3650000000000003E-2</v>
       </c>
-      <c r="C80">
-        <v>3.8792E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
         <v>5.9565E-2</v>
       </c>
-      <c r="C81">
-        <v>4.3109000000000001E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
         <v>6.5848000000000004E-2</v>
       </c>
-      <c r="C82">
-        <v>4.7800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
         <v>7.2955999999999993E-2</v>
       </c>
-      <c r="C83">
-        <v>5.3180999999999999E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84">
         <v>8.0740999999999993E-2</v>
       </c>
-      <c r="C84">
-        <v>5.9365000000000001E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
         <v>8.9357000000000006E-2</v>
       </c>
-      <c r="C85">
-        <v>6.6859000000000002E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
         <v>9.9650000000000002E-2</v>
       </c>
-      <c r="C86">
-        <v>7.5391E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
         <v>0.110901</v>
       </c>
-      <c r="C87">
-        <v>8.4744E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
         <v>0.12314600000000001</v>
       </c>
-      <c r="C88">
-        <v>9.5072000000000004E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
         <v>0.13641200000000001</v>
       </c>
-      <c r="C89">
-        <v>0.10642699999999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
         <v>0.15071000000000001</v>
       </c>
-      <c r="C90">
-        <v>0.118857</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
         <v>0.16603799999999999</v>
       </c>
-      <c r="C91">
-        <v>0.13239600000000001</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
         <v>0.18237400000000001</v>
       </c>
-      <c r="C92">
-        <v>0.147063</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
         <v>0.19967599999999999</v>
       </c>
-      <c r="C93">
-        <v>0.162859</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
         <v>0.21787999999999999</v>
       </c>
-      <c r="C94">
-        <v>0.17976500000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95">
         <v>0.236903</v>
       </c>
-      <c r="C95">
-        <v>0.197737</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96">
         <v>0.25663599999999998</v>
       </c>
-      <c r="C96">
-        <v>0.21670600000000001</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97">
         <v>0.27695399999999998</v>
       </c>
-      <c r="C97">
-        <v>0.23657700000000001</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98">
         <v>0.29771300000000001</v>
       </c>
-      <c r="C98">
-        <v>0.25722800000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
         <v>0.31875500000000001</v>
       </c>
-      <c r="C99">
-        <v>0.27851500000000001</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100">
         <v>0.33991399999999999</v>
       </c>
-      <c r="C100">
-        <v>0.30027100000000001</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
-      <c r="C101">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>3.8200000000000002E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>2.2499999999999999E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>1.75E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>1.5100000000000001E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1.3200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>1.17E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>1.06E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>9.6000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>8.7999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>8.3999999999999995E-5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>8.7000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>1.02E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>1.2899999999999999E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>1.66E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>2.0699999999999999E-4</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>2.4699999999999999E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>2.8600000000000001E-4</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>3.2000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>3.5100000000000002E-4</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>3.8400000000000001E-4</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>4.1599999999999997E-4</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>4.4499999999999997E-4</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>4.6700000000000002E-4</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>4.86E-4</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>5.0500000000000002E-4</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>5.2599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>5.53E-4</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>5.8699999999999996E-4</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>6.2699999999999995E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>6.7299999999999999E-4</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>7.2099999999999996E-4</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>7.6599999999999997E-4</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>8.0500000000000005E-4</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>8.4199999999999998E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>8.8800000000000001E-4</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>9.4700000000000003E-4</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>1.0169999999999999E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>1.0989999999999999E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1.1919999999999999E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>1.291E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>1.402E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>1.5349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>1.6949999999999999E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1.879E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>2.0699999999999998E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>2.2680000000000001E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>2.4859999999999999E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>2.725E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>2.977E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>3.2450000000000001E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>3.5140000000000002E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>3.7759999999999998E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>4.0289999999999996E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>4.2890000000000003E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>4.5640000000000003E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>4.875E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>5.2339999999999999E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>5.6470000000000001E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>6.1029999999999999E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>6.5890000000000002E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>7.1040000000000001E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>7.6649999999999999E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>8.3029999999999996E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>9.0500000000000008E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>9.953E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>1.1001E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>1.2123999999999999E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1.325E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>1.4419E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>1.5717999999999999E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>1.7201000000000001E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>1.8896E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>2.0818E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>2.2995999999999999E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>2.5387E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>2.809E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>3.1224999999999999E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>3.4785999999999997E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>3.8792E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>4.3109000000000001E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>4.7800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>5.3180999999999999E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>5.9365000000000001E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>6.6859000000000002E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>7.5391E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>8.4744E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>9.5072000000000004E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>0.10642699999999999</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>0.118857</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>0.13239600000000001</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>0.147063</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>0.162859</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>0.17976500000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>0.197737</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>0.21670600000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>0.23657700000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>0.25722800000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>0.27851500000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>0.30027100000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201">
         <v>1</v>
       </c>
     </row>
@@ -3572,10 +3801,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="5" t="s">
         <v>13</v>
       </c>

</xml_diff>